<commit_message>
Fix sample sheet active sheet bug
</commit_message>
<xml_diff>
--- a/source/portal/static/portal/excel/mng_excel_template_base.xlsx
+++ b/source/portal/static/portal/excel/mng_excel_template_base.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Lookups" sheetId="2" r:id="rId2"/>
+    <sheet name="Lookups" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Types">#REF!</definedName>
@@ -1493,7 +1493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
     </sheetView>
@@ -3758,9 +3758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5609"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Add 'Unknown' option for host/env sample type
</commit_message>
<xml_diff>
--- a/source/portal/static/portal/excel/mng_excel_template_base.xlsx
+++ b/source/portal/static/portal/excel/mng_excel_template_base.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="139">
   <si>
     <t>Geographic Location (of sample collection)</t>
   </si>
@@ -482,6 +482,9 @@
       </rPr>
       <t>Only fill in if your strain is lab derived</t>
     </r>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
 </sst>
 </file>
@@ -3756,13 +3759,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5609"/>
+  <dimension ref="B1:E5609"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
     <col min="2" max="2" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4053,6 +4058,9 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="6"/>
+      <c r="C31" t="s">
+        <v>138</v>
+      </c>
       <c r="D31" t="s">
         <v>83</v>
       </c>
@@ -4269,6 +4277,9 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B67" s="6"/>
+      <c r="D67" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B68" s="6"/>

</xml_diff>

<commit_message>
Update excel base template and form to allow entry of 0 value for dna concentration
</commit_message>
<xml_diff>
--- a/source/portal/static/portal/excel/mng_excel_template_base.xlsx
+++ b/source/portal/static/portal/excel/mng_excel_template_base.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1114,6 +1114,24 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1144,24 +1162,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1500,7 +1500,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1527,60 +1527,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="100" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
       <c r="D1" s="10"/>
       <c r="E1" s="87" t="s">
         <v>123</v>
       </c>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
       <c r="I1" s="11"/>
       <c r="J1" s="12"/>
       <c r="K1" s="13"/>
-      <c r="L1" s="102" t="s">
+      <c r="L1" s="108" t="s">
         <v>128</v>
       </c>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="103"/>
-      <c r="Q1" s="103"/>
-      <c r="R1" s="104"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="109"/>
+      <c r="O1" s="109"/>
+      <c r="P1" s="109"/>
+      <c r="Q1" s="109"/>
+      <c r="R1" s="110"/>
     </row>
     <row r="2" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="95"/>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
-      <c r="F2" s="114" t="s">
+      <c r="F2" s="99" t="s">
         <v>133</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
-      <c r="J2" s="100" t="s">
+      <c r="J2" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="101"/>
-      <c r="L2" s="98" t="s">
+      <c r="K2" s="107"/>
+      <c r="L2" s="104" t="s">
         <v>131</v>
       </c>
-      <c r="M2" s="99"/>
-      <c r="N2" s="105" t="s">
+      <c r="M2" s="105"/>
+      <c r="N2" s="111" t="s">
         <v>129</v>
       </c>
-      <c r="O2" s="106"/>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="96" t="s">
+      <c r="O2" s="112"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="102" t="s">
         <v>130</v>
       </c>
-      <c r="R2" s="97"/>
+      <c r="R2" s="103"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="65"/>
@@ -1796,7 +1796,7 @@
       <c r="C7" s="40"/>
       <c r="D7" s="41"/>
       <c r="E7" s="40"/>
-      <c r="F7" s="109"/>
+      <c r="F7" s="94"/>
       <c r="G7" s="42"/>
       <c r="H7" s="42"/>
       <c r="I7" s="74"/>
@@ -1804,7 +1804,7 @@
       <c r="K7" s="73"/>
       <c r="L7" s="47"/>
       <c r="M7" s="72"/>
-      <c r="N7" s="111"/>
+      <c r="N7" s="96"/>
       <c r="O7" s="70"/>
       <c r="P7" s="71"/>
       <c r="Q7" s="47"/>
@@ -1817,7 +1817,7 @@
       <c r="C8" s="40"/>
       <c r="D8" s="41"/>
       <c r="E8" s="40"/>
-      <c r="F8" s="109"/>
+      <c r="F8" s="94"/>
       <c r="G8" s="42"/>
       <c r="H8" s="42"/>
       <c r="I8" s="42"/>
@@ -1825,7 +1825,7 @@
       <c r="K8" s="44"/>
       <c r="L8" s="45"/>
       <c r="M8" s="46"/>
-      <c r="N8" s="112"/>
+      <c r="N8" s="97"/>
       <c r="O8" s="47"/>
       <c r="P8" s="46"/>
       <c r="Q8" s="45"/>
@@ -1837,7 +1837,7 @@
       <c r="C9" s="40"/>
       <c r="D9" s="41"/>
       <c r="E9" s="40"/>
-      <c r="F9" s="109"/>
+      <c r="F9" s="94"/>
       <c r="G9" s="42"/>
       <c r="H9" s="42"/>
       <c r="I9" s="42"/>
@@ -1845,7 +1845,7 @@
       <c r="K9" s="44"/>
       <c r="L9" s="45"/>
       <c r="M9" s="46"/>
-      <c r="N9" s="112"/>
+      <c r="N9" s="97"/>
       <c r="O9" s="47"/>
       <c r="P9" s="46"/>
       <c r="Q9" s="45"/>
@@ -1857,7 +1857,7 @@
       <c r="C10" s="40"/>
       <c r="D10" s="41"/>
       <c r="E10" s="40"/>
-      <c r="F10" s="109"/>
+      <c r="F10" s="94"/>
       <c r="G10" s="42"/>
       <c r="H10" s="42"/>
       <c r="I10" s="42"/>
@@ -1865,7 +1865,7 @@
       <c r="K10" s="44"/>
       <c r="L10" s="45"/>
       <c r="M10" s="46"/>
-      <c r="N10" s="112"/>
+      <c r="N10" s="97"/>
       <c r="O10" s="47"/>
       <c r="P10" s="46"/>
       <c r="Q10" s="45"/>
@@ -1877,7 +1877,7 @@
       <c r="C11" s="40"/>
       <c r="D11" s="41"/>
       <c r="E11" s="40"/>
-      <c r="F11" s="109"/>
+      <c r="F11" s="94"/>
       <c r="G11" s="42"/>
       <c r="H11" s="42"/>
       <c r="I11" s="42"/>
@@ -1885,7 +1885,7 @@
       <c r="K11" s="44"/>
       <c r="L11" s="45"/>
       <c r="M11" s="46"/>
-      <c r="N11" s="112"/>
+      <c r="N11" s="97"/>
       <c r="O11" s="47"/>
       <c r="P11" s="46"/>
       <c r="Q11" s="45"/>
@@ -1897,7 +1897,7 @@
       <c r="C12" s="40"/>
       <c r="D12" s="41"/>
       <c r="E12" s="40"/>
-      <c r="F12" s="109"/>
+      <c r="F12" s="94"/>
       <c r="G12" s="42"/>
       <c r="H12" s="42"/>
       <c r="I12" s="42"/>
@@ -1905,7 +1905,7 @@
       <c r="K12" s="44"/>
       <c r="L12" s="45"/>
       <c r="M12" s="46"/>
-      <c r="N12" s="112"/>
+      <c r="N12" s="97"/>
       <c r="O12" s="47"/>
       <c r="P12" s="46"/>
       <c r="Q12" s="45"/>
@@ -1917,7 +1917,7 @@
       <c r="C13" s="40"/>
       <c r="D13" s="41"/>
       <c r="E13" s="40"/>
-      <c r="F13" s="109"/>
+      <c r="F13" s="94"/>
       <c r="G13" s="42"/>
       <c r="H13" s="42"/>
       <c r="I13" s="42"/>
@@ -1925,7 +1925,7 @@
       <c r="K13" s="44"/>
       <c r="L13" s="45"/>
       <c r="M13" s="46"/>
-      <c r="N13" s="112"/>
+      <c r="N13" s="97"/>
       <c r="O13" s="47"/>
       <c r="P13" s="46"/>
       <c r="Q13" s="45"/>
@@ -1937,7 +1937,7 @@
       <c r="C14" s="40"/>
       <c r="D14" s="41"/>
       <c r="E14" s="48"/>
-      <c r="F14" s="109"/>
+      <c r="F14" s="94"/>
       <c r="G14" s="49"/>
       <c r="H14" s="49"/>
       <c r="I14" s="49"/>
@@ -1945,7 +1945,7 @@
       <c r="K14" s="51"/>
       <c r="L14" s="45"/>
       <c r="M14" s="46"/>
-      <c r="N14" s="112"/>
+      <c r="N14" s="97"/>
       <c r="O14" s="47"/>
       <c r="P14" s="46"/>
       <c r="Q14" s="45"/>
@@ -1957,7 +1957,7 @@
       <c r="C15" s="40"/>
       <c r="D15" s="41"/>
       <c r="E15" s="48"/>
-      <c r="F15" s="109"/>
+      <c r="F15" s="94"/>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
       <c r="I15" s="49"/>
@@ -1965,7 +1965,7 @@
       <c r="K15" s="51"/>
       <c r="L15" s="45"/>
       <c r="M15" s="46"/>
-      <c r="N15" s="112"/>
+      <c r="N15" s="97"/>
       <c r="O15" s="47"/>
       <c r="P15" s="46"/>
       <c r="Q15" s="45"/>
@@ -1977,7 +1977,7 @@
       <c r="C16" s="40"/>
       <c r="D16" s="41"/>
       <c r="E16" s="48"/>
-      <c r="F16" s="109"/>
+      <c r="F16" s="94"/>
       <c r="G16" s="49"/>
       <c r="H16" s="49"/>
       <c r="I16" s="49"/>
@@ -1985,7 +1985,7 @@
       <c r="K16" s="51"/>
       <c r="L16" s="45"/>
       <c r="M16" s="46"/>
-      <c r="N16" s="112"/>
+      <c r="N16" s="97"/>
       <c r="O16" s="47"/>
       <c r="P16" s="46"/>
       <c r="Q16" s="45"/>
@@ -1997,7 +1997,7 @@
       <c r="C17" s="40"/>
       <c r="D17" s="41"/>
       <c r="E17" s="48"/>
-      <c r="F17" s="109"/>
+      <c r="F17" s="94"/>
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
       <c r="I17" s="49"/>
@@ -2005,7 +2005,7 @@
       <c r="K17" s="51"/>
       <c r="L17" s="45"/>
       <c r="M17" s="46"/>
-      <c r="N17" s="112"/>
+      <c r="N17" s="97"/>
       <c r="O17" s="47"/>
       <c r="P17" s="46"/>
       <c r="Q17" s="45"/>
@@ -2017,7 +2017,7 @@
       <c r="C18" s="40"/>
       <c r="D18" s="41"/>
       <c r="E18" s="48"/>
-      <c r="F18" s="109"/>
+      <c r="F18" s="94"/>
       <c r="G18" s="49"/>
       <c r="H18" s="49"/>
       <c r="I18" s="49"/>
@@ -2025,7 +2025,7 @@
       <c r="K18" s="51"/>
       <c r="L18" s="45"/>
       <c r="M18" s="46"/>
-      <c r="N18" s="112"/>
+      <c r="N18" s="97"/>
       <c r="O18" s="47"/>
       <c r="P18" s="46"/>
       <c r="Q18" s="45"/>
@@ -2037,7 +2037,7 @@
       <c r="C19" s="40"/>
       <c r="D19" s="41"/>
       <c r="E19" s="48"/>
-      <c r="F19" s="109"/>
+      <c r="F19" s="94"/>
       <c r="G19" s="49"/>
       <c r="H19" s="49"/>
       <c r="I19" s="49"/>
@@ -2045,7 +2045,7 @@
       <c r="K19" s="51"/>
       <c r="L19" s="45"/>
       <c r="M19" s="46"/>
-      <c r="N19" s="112"/>
+      <c r="N19" s="97"/>
       <c r="O19" s="47"/>
       <c r="P19" s="46"/>
       <c r="Q19" s="45"/>
@@ -2057,7 +2057,7 @@
       <c r="C20" s="40"/>
       <c r="D20" s="41"/>
       <c r="E20" s="48"/>
-      <c r="F20" s="109"/>
+      <c r="F20" s="94"/>
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
       <c r="I20" s="49"/>
@@ -2065,7 +2065,7 @@
       <c r="K20" s="51"/>
       <c r="L20" s="45"/>
       <c r="M20" s="46"/>
-      <c r="N20" s="112"/>
+      <c r="N20" s="97"/>
       <c r="O20" s="47"/>
       <c r="P20" s="46"/>
       <c r="Q20" s="45"/>
@@ -2077,7 +2077,7 @@
       <c r="C21" s="40"/>
       <c r="D21" s="41"/>
       <c r="E21" s="48"/>
-      <c r="F21" s="109"/>
+      <c r="F21" s="94"/>
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
       <c r="I21" s="49"/>
@@ -2085,7 +2085,7 @@
       <c r="K21" s="51"/>
       <c r="L21" s="45"/>
       <c r="M21" s="46"/>
-      <c r="N21" s="112"/>
+      <c r="N21" s="97"/>
       <c r="O21" s="47"/>
       <c r="P21" s="46"/>
       <c r="Q21" s="45"/>
@@ -2097,7 +2097,7 @@
       <c r="C22" s="40"/>
       <c r="D22" s="41"/>
       <c r="E22" s="48"/>
-      <c r="F22" s="109"/>
+      <c r="F22" s="94"/>
       <c r="G22" s="49"/>
       <c r="H22" s="49"/>
       <c r="I22" s="49"/>
@@ -2105,7 +2105,7 @@
       <c r="K22" s="51"/>
       <c r="L22" s="45"/>
       <c r="M22" s="46"/>
-      <c r="N22" s="112"/>
+      <c r="N22" s="97"/>
       <c r="O22" s="47"/>
       <c r="P22" s="46"/>
       <c r="Q22" s="45"/>
@@ -2117,7 +2117,7 @@
       <c r="C23" s="40"/>
       <c r="D23" s="41"/>
       <c r="E23" s="48"/>
-      <c r="F23" s="109"/>
+      <c r="F23" s="94"/>
       <c r="G23" s="49"/>
       <c r="H23" s="49"/>
       <c r="I23" s="49"/>
@@ -2125,7 +2125,7 @@
       <c r="K23" s="51"/>
       <c r="L23" s="45"/>
       <c r="M23" s="46"/>
-      <c r="N23" s="112"/>
+      <c r="N23" s="97"/>
       <c r="O23" s="47"/>
       <c r="P23" s="46"/>
       <c r="Q23" s="45"/>
@@ -2137,7 +2137,7 @@
       <c r="C24" s="40"/>
       <c r="D24" s="41"/>
       <c r="E24" s="48"/>
-      <c r="F24" s="109"/>
+      <c r="F24" s="94"/>
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
       <c r="I24" s="49"/>
@@ -2145,7 +2145,7 @@
       <c r="K24" s="51"/>
       <c r="L24" s="45"/>
       <c r="M24" s="46"/>
-      <c r="N24" s="112"/>
+      <c r="N24" s="97"/>
       <c r="O24" s="47"/>
       <c r="P24" s="46"/>
       <c r="Q24" s="45"/>
@@ -2157,7 +2157,7 @@
       <c r="C25" s="40"/>
       <c r="D25" s="41"/>
       <c r="E25" s="48"/>
-      <c r="F25" s="109"/>
+      <c r="F25" s="94"/>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
       <c r="I25" s="49"/>
@@ -2165,7 +2165,7 @@
       <c r="K25" s="51"/>
       <c r="L25" s="45"/>
       <c r="M25" s="46"/>
-      <c r="N25" s="112"/>
+      <c r="N25" s="97"/>
       <c r="O25" s="47"/>
       <c r="P25" s="46"/>
       <c r="Q25" s="45"/>
@@ -2177,7 +2177,7 @@
       <c r="C26" s="40"/>
       <c r="D26" s="41"/>
       <c r="E26" s="48"/>
-      <c r="F26" s="109"/>
+      <c r="F26" s="94"/>
       <c r="G26" s="49"/>
       <c r="H26" s="49"/>
       <c r="I26" s="49"/>
@@ -2185,7 +2185,7 @@
       <c r="K26" s="51"/>
       <c r="L26" s="45"/>
       <c r="M26" s="46"/>
-      <c r="N26" s="112"/>
+      <c r="N26" s="97"/>
       <c r="O26" s="47"/>
       <c r="P26" s="46"/>
       <c r="Q26" s="45"/>
@@ -2197,7 +2197,7 @@
       <c r="C27" s="40"/>
       <c r="D27" s="41"/>
       <c r="E27" s="48"/>
-      <c r="F27" s="109"/>
+      <c r="F27" s="94"/>
       <c r="G27" s="49"/>
       <c r="H27" s="49"/>
       <c r="I27" s="49"/>
@@ -2205,7 +2205,7 @@
       <c r="K27" s="51"/>
       <c r="L27" s="45"/>
       <c r="M27" s="46"/>
-      <c r="N27" s="112"/>
+      <c r="N27" s="97"/>
       <c r="O27" s="47"/>
       <c r="P27" s="46"/>
       <c r="Q27" s="45"/>
@@ -2217,7 +2217,7 @@
       <c r="C28" s="40"/>
       <c r="D28" s="41"/>
       <c r="E28" s="48"/>
-      <c r="F28" s="109"/>
+      <c r="F28" s="94"/>
       <c r="G28" s="49"/>
       <c r="H28" s="49"/>
       <c r="I28" s="49"/>
@@ -2225,7 +2225,7 @@
       <c r="K28" s="51"/>
       <c r="L28" s="45"/>
       <c r="M28" s="46"/>
-      <c r="N28" s="112"/>
+      <c r="N28" s="97"/>
       <c r="O28" s="47"/>
       <c r="P28" s="46"/>
       <c r="Q28" s="45"/>
@@ -2237,7 +2237,7 @@
       <c r="C29" s="40"/>
       <c r="D29" s="41"/>
       <c r="E29" s="48"/>
-      <c r="F29" s="109"/>
+      <c r="F29" s="94"/>
       <c r="G29" s="49"/>
       <c r="H29" s="49"/>
       <c r="I29" s="49"/>
@@ -2245,7 +2245,7 @@
       <c r="K29" s="51"/>
       <c r="L29" s="45"/>
       <c r="M29" s="46"/>
-      <c r="N29" s="112"/>
+      <c r="N29" s="97"/>
       <c r="O29" s="47"/>
       <c r="P29" s="46"/>
       <c r="Q29" s="45"/>
@@ -2257,7 +2257,7 @@
       <c r="C30" s="40"/>
       <c r="D30" s="41"/>
       <c r="E30" s="48"/>
-      <c r="F30" s="109"/>
+      <c r="F30" s="94"/>
       <c r="G30" s="49"/>
       <c r="H30" s="49"/>
       <c r="I30" s="49"/>
@@ -2265,7 +2265,7 @@
       <c r="K30" s="51"/>
       <c r="L30" s="45"/>
       <c r="M30" s="46"/>
-      <c r="N30" s="112"/>
+      <c r="N30" s="97"/>
       <c r="O30" s="47"/>
       <c r="P30" s="46"/>
       <c r="Q30" s="45"/>
@@ -2277,7 +2277,7 @@
       <c r="C31" s="40"/>
       <c r="D31" s="41"/>
       <c r="E31" s="48"/>
-      <c r="F31" s="109"/>
+      <c r="F31" s="94"/>
       <c r="G31" s="49"/>
       <c r="H31" s="49"/>
       <c r="I31" s="49"/>
@@ -2285,7 +2285,7 @@
       <c r="K31" s="51"/>
       <c r="L31" s="45"/>
       <c r="M31" s="46"/>
-      <c r="N31" s="112"/>
+      <c r="N31" s="97"/>
       <c r="O31" s="47"/>
       <c r="P31" s="46"/>
       <c r="Q31" s="45"/>
@@ -2297,7 +2297,7 @@
       <c r="C32" s="40"/>
       <c r="D32" s="41"/>
       <c r="E32" s="48"/>
-      <c r="F32" s="109"/>
+      <c r="F32" s="94"/>
       <c r="G32" s="49"/>
       <c r="H32" s="49"/>
       <c r="I32" s="49"/>
@@ -2305,7 +2305,7 @@
       <c r="K32" s="51"/>
       <c r="L32" s="45"/>
       <c r="M32" s="46"/>
-      <c r="N32" s="112"/>
+      <c r="N32" s="97"/>
       <c r="O32" s="47"/>
       <c r="P32" s="46"/>
       <c r="Q32" s="45"/>
@@ -2317,7 +2317,7 @@
       <c r="C33" s="40"/>
       <c r="D33" s="41"/>
       <c r="E33" s="48"/>
-      <c r="F33" s="109"/>
+      <c r="F33" s="94"/>
       <c r="G33" s="49"/>
       <c r="H33" s="49"/>
       <c r="I33" s="49"/>
@@ -2325,7 +2325,7 @@
       <c r="K33" s="51"/>
       <c r="L33" s="45"/>
       <c r="M33" s="46"/>
-      <c r="N33" s="112"/>
+      <c r="N33" s="97"/>
       <c r="O33" s="47"/>
       <c r="P33" s="46"/>
       <c r="Q33" s="45"/>
@@ -2337,7 +2337,7 @@
       <c r="C34" s="40"/>
       <c r="D34" s="41"/>
       <c r="E34" s="48"/>
-      <c r="F34" s="109"/>
+      <c r="F34" s="94"/>
       <c r="G34" s="49"/>
       <c r="H34" s="49"/>
       <c r="I34" s="49"/>
@@ -2345,7 +2345,7 @@
       <c r="K34" s="51"/>
       <c r="L34" s="45"/>
       <c r="M34" s="46"/>
-      <c r="N34" s="112"/>
+      <c r="N34" s="97"/>
       <c r="O34" s="47"/>
       <c r="P34" s="46"/>
       <c r="Q34" s="45"/>
@@ -2357,7 +2357,7 @@
       <c r="C35" s="40"/>
       <c r="D35" s="41"/>
       <c r="E35" s="48"/>
-      <c r="F35" s="109"/>
+      <c r="F35" s="94"/>
       <c r="G35" s="49"/>
       <c r="H35" s="49"/>
       <c r="I35" s="49"/>
@@ -2365,7 +2365,7 @@
       <c r="K35" s="51"/>
       <c r="L35" s="45"/>
       <c r="M35" s="46"/>
-      <c r="N35" s="112"/>
+      <c r="N35" s="97"/>
       <c r="O35" s="47"/>
       <c r="P35" s="46"/>
       <c r="Q35" s="45"/>
@@ -2377,7 +2377,7 @@
       <c r="C36" s="40"/>
       <c r="D36" s="41"/>
       <c r="E36" s="48"/>
-      <c r="F36" s="109"/>
+      <c r="F36" s="94"/>
       <c r="G36" s="49"/>
       <c r="H36" s="49"/>
       <c r="I36" s="49"/>
@@ -2385,7 +2385,7 @@
       <c r="K36" s="51"/>
       <c r="L36" s="45"/>
       <c r="M36" s="46"/>
-      <c r="N36" s="112"/>
+      <c r="N36" s="97"/>
       <c r="O36" s="47"/>
       <c r="P36" s="46"/>
       <c r="Q36" s="45"/>
@@ -2397,7 +2397,7 @@
       <c r="C37" s="40"/>
       <c r="D37" s="41"/>
       <c r="E37" s="48"/>
-      <c r="F37" s="109"/>
+      <c r="F37" s="94"/>
       <c r="G37" s="49"/>
       <c r="H37" s="49"/>
       <c r="I37" s="49"/>
@@ -2405,7 +2405,7 @@
       <c r="K37" s="51"/>
       <c r="L37" s="45"/>
       <c r="M37" s="46"/>
-      <c r="N37" s="112"/>
+      <c r="N37" s="97"/>
       <c r="O37" s="47"/>
       <c r="P37" s="46"/>
       <c r="Q37" s="45"/>
@@ -2417,7 +2417,7 @@
       <c r="C38" s="40"/>
       <c r="D38" s="41"/>
       <c r="E38" s="48"/>
-      <c r="F38" s="109"/>
+      <c r="F38" s="94"/>
       <c r="G38" s="49"/>
       <c r="H38" s="49"/>
       <c r="I38" s="49"/>
@@ -2425,7 +2425,7 @@
       <c r="K38" s="51"/>
       <c r="L38" s="45"/>
       <c r="M38" s="46"/>
-      <c r="N38" s="112"/>
+      <c r="N38" s="97"/>
       <c r="O38" s="47"/>
       <c r="P38" s="46"/>
       <c r="Q38" s="45"/>
@@ -2437,7 +2437,7 @@
       <c r="C39" s="40"/>
       <c r="D39" s="41"/>
       <c r="E39" s="48"/>
-      <c r="F39" s="109"/>
+      <c r="F39" s="94"/>
       <c r="G39" s="49"/>
       <c r="H39" s="49"/>
       <c r="I39" s="49"/>
@@ -2445,7 +2445,7 @@
       <c r="K39" s="51"/>
       <c r="L39" s="45"/>
       <c r="M39" s="46"/>
-      <c r="N39" s="112"/>
+      <c r="N39" s="97"/>
       <c r="O39" s="47"/>
       <c r="P39" s="46"/>
       <c r="Q39" s="45"/>
@@ -2457,7 +2457,7 @@
       <c r="C40" s="40"/>
       <c r="D40" s="41"/>
       <c r="E40" s="48"/>
-      <c r="F40" s="109"/>
+      <c r="F40" s="94"/>
       <c r="G40" s="49"/>
       <c r="H40" s="49"/>
       <c r="I40" s="49"/>
@@ -2465,7 +2465,7 @@
       <c r="K40" s="51"/>
       <c r="L40" s="45"/>
       <c r="M40" s="46"/>
-      <c r="N40" s="112"/>
+      <c r="N40" s="97"/>
       <c r="O40" s="47"/>
       <c r="P40" s="46"/>
       <c r="Q40" s="45"/>
@@ -2477,7 +2477,7 @@
       <c r="C41" s="40"/>
       <c r="D41" s="41"/>
       <c r="E41" s="48"/>
-      <c r="F41" s="109"/>
+      <c r="F41" s="94"/>
       <c r="G41" s="49"/>
       <c r="H41" s="49"/>
       <c r="I41" s="49"/>
@@ -2485,7 +2485,7 @@
       <c r="K41" s="51"/>
       <c r="L41" s="45"/>
       <c r="M41" s="46"/>
-      <c r="N41" s="112"/>
+      <c r="N41" s="97"/>
       <c r="O41" s="47"/>
       <c r="P41" s="46"/>
       <c r="Q41" s="45"/>
@@ -2497,7 +2497,7 @@
       <c r="C42" s="40"/>
       <c r="D42" s="41"/>
       <c r="E42" s="48"/>
-      <c r="F42" s="109"/>
+      <c r="F42" s="94"/>
       <c r="G42" s="49"/>
       <c r="H42" s="49"/>
       <c r="I42" s="49"/>
@@ -2505,7 +2505,7 @@
       <c r="K42" s="51"/>
       <c r="L42" s="45"/>
       <c r="M42" s="46"/>
-      <c r="N42" s="112"/>
+      <c r="N42" s="97"/>
       <c r="O42" s="47"/>
       <c r="P42" s="46"/>
       <c r="Q42" s="45"/>
@@ -2517,7 +2517,7 @@
       <c r="C43" s="40"/>
       <c r="D43" s="41"/>
       <c r="E43" s="48"/>
-      <c r="F43" s="109"/>
+      <c r="F43" s="94"/>
       <c r="G43" s="49"/>
       <c r="H43" s="49"/>
       <c r="I43" s="49"/>
@@ -2525,7 +2525,7 @@
       <c r="K43" s="51"/>
       <c r="L43" s="45"/>
       <c r="M43" s="46"/>
-      <c r="N43" s="112"/>
+      <c r="N43" s="97"/>
       <c r="O43" s="47"/>
       <c r="P43" s="46"/>
       <c r="Q43" s="45"/>
@@ -2537,7 +2537,7 @@
       <c r="C44" s="40"/>
       <c r="D44" s="41"/>
       <c r="E44" s="48"/>
-      <c r="F44" s="109"/>
+      <c r="F44" s="94"/>
       <c r="G44" s="49"/>
       <c r="H44" s="49"/>
       <c r="I44" s="49"/>
@@ -2545,7 +2545,7 @@
       <c r="K44" s="51"/>
       <c r="L44" s="45"/>
       <c r="M44" s="46"/>
-      <c r="N44" s="112"/>
+      <c r="N44" s="97"/>
       <c r="O44" s="47"/>
       <c r="P44" s="46"/>
       <c r="Q44" s="45"/>
@@ -2557,7 +2557,7 @@
       <c r="C45" s="40"/>
       <c r="D45" s="41"/>
       <c r="E45" s="48"/>
-      <c r="F45" s="109"/>
+      <c r="F45" s="94"/>
       <c r="G45" s="49"/>
       <c r="H45" s="49"/>
       <c r="I45" s="49"/>
@@ -2565,7 +2565,7 @@
       <c r="K45" s="51"/>
       <c r="L45" s="45"/>
       <c r="M45" s="46"/>
-      <c r="N45" s="112"/>
+      <c r="N45" s="97"/>
       <c r="O45" s="47"/>
       <c r="P45" s="46"/>
       <c r="Q45" s="45"/>
@@ -2577,7 +2577,7 @@
       <c r="C46" s="40"/>
       <c r="D46" s="41"/>
       <c r="E46" s="48"/>
-      <c r="F46" s="109"/>
+      <c r="F46" s="94"/>
       <c r="G46" s="49"/>
       <c r="H46" s="49"/>
       <c r="I46" s="49"/>
@@ -2585,7 +2585,7 @@
       <c r="K46" s="51"/>
       <c r="L46" s="45"/>
       <c r="M46" s="46"/>
-      <c r="N46" s="112"/>
+      <c r="N46" s="97"/>
       <c r="O46" s="47"/>
       <c r="P46" s="46"/>
       <c r="Q46" s="45"/>
@@ -2597,7 +2597,7 @@
       <c r="C47" s="40"/>
       <c r="D47" s="41"/>
       <c r="E47" s="48"/>
-      <c r="F47" s="109"/>
+      <c r="F47" s="94"/>
       <c r="G47" s="49"/>
       <c r="H47" s="49"/>
       <c r="I47" s="49"/>
@@ -2605,7 +2605,7 @@
       <c r="K47" s="51"/>
       <c r="L47" s="45"/>
       <c r="M47" s="46"/>
-      <c r="N47" s="112"/>
+      <c r="N47" s="97"/>
       <c r="O47" s="47"/>
       <c r="P47" s="46"/>
       <c r="Q47" s="45"/>
@@ -2617,7 +2617,7 @@
       <c r="C48" s="40"/>
       <c r="D48" s="41"/>
       <c r="E48" s="48"/>
-      <c r="F48" s="109"/>
+      <c r="F48" s="94"/>
       <c r="G48" s="49"/>
       <c r="H48" s="49"/>
       <c r="I48" s="49"/>
@@ -2625,7 +2625,7 @@
       <c r="K48" s="51"/>
       <c r="L48" s="45"/>
       <c r="M48" s="46"/>
-      <c r="N48" s="112"/>
+      <c r="N48" s="97"/>
       <c r="O48" s="47"/>
       <c r="P48" s="46"/>
       <c r="Q48" s="45"/>
@@ -2637,7 +2637,7 @@
       <c r="C49" s="40"/>
       <c r="D49" s="41"/>
       <c r="E49" s="48"/>
-      <c r="F49" s="109"/>
+      <c r="F49" s="94"/>
       <c r="G49" s="49"/>
       <c r="H49" s="49"/>
       <c r="I49" s="49"/>
@@ -2645,7 +2645,7 @@
       <c r="K49" s="51"/>
       <c r="L49" s="45"/>
       <c r="M49" s="46"/>
-      <c r="N49" s="112"/>
+      <c r="N49" s="97"/>
       <c r="O49" s="47"/>
       <c r="P49" s="46"/>
       <c r="Q49" s="45"/>
@@ -2657,7 +2657,7 @@
       <c r="C50" s="40"/>
       <c r="D50" s="41"/>
       <c r="E50" s="48"/>
-      <c r="F50" s="109"/>
+      <c r="F50" s="94"/>
       <c r="G50" s="49"/>
       <c r="H50" s="49"/>
       <c r="I50" s="49"/>
@@ -2665,7 +2665,7 @@
       <c r="K50" s="51"/>
       <c r="L50" s="45"/>
       <c r="M50" s="46"/>
-      <c r="N50" s="112"/>
+      <c r="N50" s="97"/>
       <c r="O50" s="47"/>
       <c r="P50" s="46"/>
       <c r="Q50" s="45"/>
@@ -2677,7 +2677,7 @@
       <c r="C51" s="40"/>
       <c r="D51" s="41"/>
       <c r="E51" s="48"/>
-      <c r="F51" s="109"/>
+      <c r="F51" s="94"/>
       <c r="G51" s="49"/>
       <c r="H51" s="49"/>
       <c r="I51" s="49"/>
@@ -2685,7 +2685,7 @@
       <c r="K51" s="51"/>
       <c r="L51" s="45"/>
       <c r="M51" s="46"/>
-      <c r="N51" s="112"/>
+      <c r="N51" s="97"/>
       <c r="O51" s="47"/>
       <c r="P51" s="46"/>
       <c r="Q51" s="45"/>
@@ -2697,7 +2697,7 @@
       <c r="C52" s="40"/>
       <c r="D52" s="41"/>
       <c r="E52" s="48"/>
-      <c r="F52" s="109"/>
+      <c r="F52" s="94"/>
       <c r="G52" s="49"/>
       <c r="H52" s="49"/>
       <c r="I52" s="49"/>
@@ -2705,7 +2705,7 @@
       <c r="K52" s="51"/>
       <c r="L52" s="45"/>
       <c r="M52" s="46"/>
-      <c r="N52" s="112"/>
+      <c r="N52" s="97"/>
       <c r="O52" s="47"/>
       <c r="P52" s="46"/>
       <c r="Q52" s="45"/>
@@ -2717,7 +2717,7 @@
       <c r="C53" s="40"/>
       <c r="D53" s="41"/>
       <c r="E53" s="48"/>
-      <c r="F53" s="109"/>
+      <c r="F53" s="94"/>
       <c r="G53" s="49"/>
       <c r="H53" s="49"/>
       <c r="I53" s="49"/>
@@ -2725,7 +2725,7 @@
       <c r="K53" s="51"/>
       <c r="L53" s="45"/>
       <c r="M53" s="46"/>
-      <c r="N53" s="112"/>
+      <c r="N53" s="97"/>
       <c r="O53" s="47"/>
       <c r="P53" s="46"/>
       <c r="Q53" s="45"/>
@@ -2737,7 +2737,7 @@
       <c r="C54" s="40"/>
       <c r="D54" s="41"/>
       <c r="E54" s="48"/>
-      <c r="F54" s="109"/>
+      <c r="F54" s="94"/>
       <c r="G54" s="49"/>
       <c r="H54" s="49"/>
       <c r="I54" s="49"/>
@@ -2745,7 +2745,7 @@
       <c r="K54" s="51"/>
       <c r="L54" s="45"/>
       <c r="M54" s="46"/>
-      <c r="N54" s="112"/>
+      <c r="N54" s="97"/>
       <c r="O54" s="47"/>
       <c r="P54" s="46"/>
       <c r="Q54" s="45"/>
@@ -2757,7 +2757,7 @@
       <c r="C55" s="40"/>
       <c r="D55" s="41"/>
       <c r="E55" s="48"/>
-      <c r="F55" s="109"/>
+      <c r="F55" s="94"/>
       <c r="G55" s="49"/>
       <c r="H55" s="49"/>
       <c r="I55" s="49"/>
@@ -2765,7 +2765,7 @@
       <c r="K55" s="51"/>
       <c r="L55" s="45"/>
       <c r="M55" s="46"/>
-      <c r="N55" s="112"/>
+      <c r="N55" s="97"/>
       <c r="O55" s="47"/>
       <c r="P55" s="46"/>
       <c r="Q55" s="45"/>
@@ -2777,7 +2777,7 @@
       <c r="C56" s="40"/>
       <c r="D56" s="41"/>
       <c r="E56" s="48"/>
-      <c r="F56" s="109"/>
+      <c r="F56" s="94"/>
       <c r="G56" s="49"/>
       <c r="H56" s="49"/>
       <c r="I56" s="49"/>
@@ -2785,7 +2785,7 @@
       <c r="K56" s="51"/>
       <c r="L56" s="45"/>
       <c r="M56" s="46"/>
-      <c r="N56" s="112"/>
+      <c r="N56" s="97"/>
       <c r="O56" s="47"/>
       <c r="P56" s="46"/>
       <c r="Q56" s="45"/>
@@ -2797,7 +2797,7 @@
       <c r="C57" s="40"/>
       <c r="D57" s="41"/>
       <c r="E57" s="48"/>
-      <c r="F57" s="109"/>
+      <c r="F57" s="94"/>
       <c r="G57" s="49"/>
       <c r="H57" s="49"/>
       <c r="I57" s="49"/>
@@ -2805,7 +2805,7 @@
       <c r="K57" s="51"/>
       <c r="L57" s="45"/>
       <c r="M57" s="46"/>
-      <c r="N57" s="112"/>
+      <c r="N57" s="97"/>
       <c r="O57" s="47"/>
       <c r="P57" s="46"/>
       <c r="Q57" s="45"/>
@@ -2817,7 +2817,7 @@
       <c r="C58" s="40"/>
       <c r="D58" s="41"/>
       <c r="E58" s="48"/>
-      <c r="F58" s="109"/>
+      <c r="F58" s="94"/>
       <c r="G58" s="49"/>
       <c r="H58" s="49"/>
       <c r="I58" s="49"/>
@@ -2825,7 +2825,7 @@
       <c r="K58" s="51"/>
       <c r="L58" s="45"/>
       <c r="M58" s="46"/>
-      <c r="N58" s="112"/>
+      <c r="N58" s="97"/>
       <c r="O58" s="47"/>
       <c r="P58" s="46"/>
       <c r="Q58" s="45"/>
@@ -2837,7 +2837,7 @@
       <c r="C59" s="40"/>
       <c r="D59" s="41"/>
       <c r="E59" s="48"/>
-      <c r="F59" s="109"/>
+      <c r="F59" s="94"/>
       <c r="G59" s="49"/>
       <c r="H59" s="49"/>
       <c r="I59" s="49"/>
@@ -2845,7 +2845,7 @@
       <c r="K59" s="51"/>
       <c r="L59" s="45"/>
       <c r="M59" s="46"/>
-      <c r="N59" s="112"/>
+      <c r="N59" s="97"/>
       <c r="O59" s="47"/>
       <c r="P59" s="46"/>
       <c r="Q59" s="45"/>
@@ -2857,7 +2857,7 @@
       <c r="C60" s="40"/>
       <c r="D60" s="41"/>
       <c r="E60" s="48"/>
-      <c r="F60" s="109"/>
+      <c r="F60" s="94"/>
       <c r="G60" s="49"/>
       <c r="H60" s="49"/>
       <c r="I60" s="49"/>
@@ -2865,7 +2865,7 @@
       <c r="K60" s="51"/>
       <c r="L60" s="45"/>
       <c r="M60" s="46"/>
-      <c r="N60" s="112"/>
+      <c r="N60" s="97"/>
       <c r="O60" s="47"/>
       <c r="P60" s="46"/>
       <c r="Q60" s="45"/>
@@ -2877,7 +2877,7 @@
       <c r="C61" s="40"/>
       <c r="D61" s="41"/>
       <c r="E61" s="48"/>
-      <c r="F61" s="109"/>
+      <c r="F61" s="94"/>
       <c r="G61" s="49"/>
       <c r="H61" s="49"/>
       <c r="I61" s="49"/>
@@ -2885,7 +2885,7 @@
       <c r="K61" s="51"/>
       <c r="L61" s="45"/>
       <c r="M61" s="46"/>
-      <c r="N61" s="112"/>
+      <c r="N61" s="97"/>
       <c r="O61" s="47"/>
       <c r="P61" s="46"/>
       <c r="Q61" s="45"/>
@@ -2897,7 +2897,7 @@
       <c r="C62" s="40"/>
       <c r="D62" s="41"/>
       <c r="E62" s="48"/>
-      <c r="F62" s="109"/>
+      <c r="F62" s="94"/>
       <c r="G62" s="49"/>
       <c r="H62" s="49"/>
       <c r="I62" s="49"/>
@@ -2905,7 +2905,7 @@
       <c r="K62" s="51"/>
       <c r="L62" s="45"/>
       <c r="M62" s="46"/>
-      <c r="N62" s="112"/>
+      <c r="N62" s="97"/>
       <c r="O62" s="47"/>
       <c r="P62" s="46"/>
       <c r="Q62" s="45"/>
@@ -2917,7 +2917,7 @@
       <c r="C63" s="40"/>
       <c r="D63" s="41"/>
       <c r="E63" s="48"/>
-      <c r="F63" s="109"/>
+      <c r="F63" s="94"/>
       <c r="G63" s="49"/>
       <c r="H63" s="49"/>
       <c r="I63" s="49"/>
@@ -2925,7 +2925,7 @@
       <c r="K63" s="51"/>
       <c r="L63" s="45"/>
       <c r="M63" s="46"/>
-      <c r="N63" s="112"/>
+      <c r="N63" s="97"/>
       <c r="O63" s="47"/>
       <c r="P63" s="46"/>
       <c r="Q63" s="45"/>
@@ -2937,7 +2937,7 @@
       <c r="C64" s="40"/>
       <c r="D64" s="41"/>
       <c r="E64" s="48"/>
-      <c r="F64" s="109"/>
+      <c r="F64" s="94"/>
       <c r="G64" s="49"/>
       <c r="H64" s="49"/>
       <c r="I64" s="49"/>
@@ -2945,7 +2945,7 @@
       <c r="K64" s="51"/>
       <c r="L64" s="45"/>
       <c r="M64" s="46"/>
-      <c r="N64" s="112"/>
+      <c r="N64" s="97"/>
       <c r="O64" s="47"/>
       <c r="P64" s="46"/>
       <c r="Q64" s="45"/>
@@ -2957,7 +2957,7 @@
       <c r="C65" s="40"/>
       <c r="D65" s="41"/>
       <c r="E65" s="48"/>
-      <c r="F65" s="109"/>
+      <c r="F65" s="94"/>
       <c r="G65" s="49"/>
       <c r="H65" s="49"/>
       <c r="I65" s="49"/>
@@ -2965,7 +2965,7 @@
       <c r="K65" s="51"/>
       <c r="L65" s="45"/>
       <c r="M65" s="46"/>
-      <c r="N65" s="112"/>
+      <c r="N65" s="97"/>
       <c r="O65" s="47"/>
       <c r="P65" s="46"/>
       <c r="Q65" s="45"/>
@@ -2977,7 +2977,7 @@
       <c r="C66" s="40"/>
       <c r="D66" s="41"/>
       <c r="E66" s="48"/>
-      <c r="F66" s="109"/>
+      <c r="F66" s="94"/>
       <c r="G66" s="49"/>
       <c r="H66" s="49"/>
       <c r="I66" s="49"/>
@@ -2985,7 +2985,7 @@
       <c r="K66" s="51"/>
       <c r="L66" s="45"/>
       <c r="M66" s="46"/>
-      <c r="N66" s="112"/>
+      <c r="N66" s="97"/>
       <c r="O66" s="47"/>
       <c r="P66" s="46"/>
       <c r="Q66" s="45"/>
@@ -2997,7 +2997,7 @@
       <c r="C67" s="40"/>
       <c r="D67" s="41"/>
       <c r="E67" s="48"/>
-      <c r="F67" s="109"/>
+      <c r="F67" s="94"/>
       <c r="G67" s="49"/>
       <c r="H67" s="49"/>
       <c r="I67" s="49"/>
@@ -3005,7 +3005,7 @@
       <c r="K67" s="51"/>
       <c r="L67" s="45"/>
       <c r="M67" s="46"/>
-      <c r="N67" s="112"/>
+      <c r="N67" s="97"/>
       <c r="O67" s="47"/>
       <c r="P67" s="46"/>
       <c r="Q67" s="45"/>
@@ -3017,7 +3017,7 @@
       <c r="C68" s="40"/>
       <c r="D68" s="41"/>
       <c r="E68" s="48"/>
-      <c r="F68" s="109"/>
+      <c r="F68" s="94"/>
       <c r="G68" s="49"/>
       <c r="H68" s="49"/>
       <c r="I68" s="49"/>
@@ -3025,7 +3025,7 @@
       <c r="K68" s="51"/>
       <c r="L68" s="45"/>
       <c r="M68" s="46"/>
-      <c r="N68" s="112"/>
+      <c r="N68" s="97"/>
       <c r="O68" s="47"/>
       <c r="P68" s="46"/>
       <c r="Q68" s="45"/>
@@ -3037,7 +3037,7 @@
       <c r="C69" s="40"/>
       <c r="D69" s="41"/>
       <c r="E69" s="48"/>
-      <c r="F69" s="109"/>
+      <c r="F69" s="94"/>
       <c r="G69" s="49"/>
       <c r="H69" s="49"/>
       <c r="I69" s="49"/>
@@ -3045,7 +3045,7 @@
       <c r="K69" s="51"/>
       <c r="L69" s="45"/>
       <c r="M69" s="46"/>
-      <c r="N69" s="112"/>
+      <c r="N69" s="97"/>
       <c r="O69" s="47"/>
       <c r="P69" s="46"/>
       <c r="Q69" s="45"/>
@@ -3057,7 +3057,7 @@
       <c r="C70" s="40"/>
       <c r="D70" s="41"/>
       <c r="E70" s="48"/>
-      <c r="F70" s="109"/>
+      <c r="F70" s="94"/>
       <c r="G70" s="49"/>
       <c r="H70" s="49"/>
       <c r="I70" s="49"/>
@@ -3065,7 +3065,7 @@
       <c r="K70" s="51"/>
       <c r="L70" s="45"/>
       <c r="M70" s="46"/>
-      <c r="N70" s="112"/>
+      <c r="N70" s="97"/>
       <c r="O70" s="47"/>
       <c r="P70" s="46"/>
       <c r="Q70" s="45"/>
@@ -3077,7 +3077,7 @@
       <c r="C71" s="40"/>
       <c r="D71" s="41"/>
       <c r="E71" s="48"/>
-      <c r="F71" s="109"/>
+      <c r="F71" s="94"/>
       <c r="G71" s="49"/>
       <c r="H71" s="49"/>
       <c r="I71" s="49"/>
@@ -3085,7 +3085,7 @@
       <c r="K71" s="51"/>
       <c r="L71" s="45"/>
       <c r="M71" s="46"/>
-      <c r="N71" s="112"/>
+      <c r="N71" s="97"/>
       <c r="O71" s="47"/>
       <c r="P71" s="46"/>
       <c r="Q71" s="45"/>
@@ -3097,7 +3097,7 @@
       <c r="C72" s="40"/>
       <c r="D72" s="41"/>
       <c r="E72" s="48"/>
-      <c r="F72" s="109"/>
+      <c r="F72" s="94"/>
       <c r="G72" s="49"/>
       <c r="H72" s="49"/>
       <c r="I72" s="49"/>
@@ -3105,7 +3105,7 @@
       <c r="K72" s="51"/>
       <c r="L72" s="45"/>
       <c r="M72" s="46"/>
-      <c r="N72" s="112"/>
+      <c r="N72" s="97"/>
       <c r="O72" s="47"/>
       <c r="P72" s="46"/>
       <c r="Q72" s="45"/>
@@ -3117,7 +3117,7 @@
       <c r="C73" s="40"/>
       <c r="D73" s="41"/>
       <c r="E73" s="48"/>
-      <c r="F73" s="109"/>
+      <c r="F73" s="94"/>
       <c r="G73" s="49"/>
       <c r="H73" s="49"/>
       <c r="I73" s="49"/>
@@ -3125,7 +3125,7 @@
       <c r="K73" s="51"/>
       <c r="L73" s="45"/>
       <c r="M73" s="46"/>
-      <c r="N73" s="112"/>
+      <c r="N73" s="97"/>
       <c r="O73" s="47"/>
       <c r="P73" s="46"/>
       <c r="Q73" s="45"/>
@@ -3137,7 +3137,7 @@
       <c r="C74" s="40"/>
       <c r="D74" s="41"/>
       <c r="E74" s="48"/>
-      <c r="F74" s="109"/>
+      <c r="F74" s="94"/>
       <c r="G74" s="49"/>
       <c r="H74" s="49"/>
       <c r="I74" s="49"/>
@@ -3145,7 +3145,7 @@
       <c r="K74" s="51"/>
       <c r="L74" s="45"/>
       <c r="M74" s="46"/>
-      <c r="N74" s="112"/>
+      <c r="N74" s="97"/>
       <c r="O74" s="47"/>
       <c r="P74" s="46"/>
       <c r="Q74" s="45"/>
@@ -3157,7 +3157,7 @@
       <c r="C75" s="40"/>
       <c r="D75" s="41"/>
       <c r="E75" s="48"/>
-      <c r="F75" s="109"/>
+      <c r="F75" s="94"/>
       <c r="G75" s="49"/>
       <c r="H75" s="49"/>
       <c r="I75" s="49"/>
@@ -3165,7 +3165,7 @@
       <c r="K75" s="51"/>
       <c r="L75" s="45"/>
       <c r="M75" s="46"/>
-      <c r="N75" s="112"/>
+      <c r="N75" s="97"/>
       <c r="O75" s="47"/>
       <c r="P75" s="46"/>
       <c r="Q75" s="45"/>
@@ -3177,7 +3177,7 @@
       <c r="C76" s="40"/>
       <c r="D76" s="41"/>
       <c r="E76" s="48"/>
-      <c r="F76" s="109"/>
+      <c r="F76" s="94"/>
       <c r="G76" s="49"/>
       <c r="H76" s="49"/>
       <c r="I76" s="49"/>
@@ -3185,7 +3185,7 @@
       <c r="K76" s="51"/>
       <c r="L76" s="45"/>
       <c r="M76" s="46"/>
-      <c r="N76" s="112"/>
+      <c r="N76" s="97"/>
       <c r="O76" s="47"/>
       <c r="P76" s="46"/>
       <c r="Q76" s="45"/>
@@ -3197,7 +3197,7 @@
       <c r="C77" s="40"/>
       <c r="D77" s="41"/>
       <c r="E77" s="48"/>
-      <c r="F77" s="109"/>
+      <c r="F77" s="94"/>
       <c r="G77" s="49"/>
       <c r="H77" s="49"/>
       <c r="I77" s="49"/>
@@ -3205,7 +3205,7 @@
       <c r="K77" s="51"/>
       <c r="L77" s="45"/>
       <c r="M77" s="46"/>
-      <c r="N77" s="112"/>
+      <c r="N77" s="97"/>
       <c r="O77" s="47"/>
       <c r="P77" s="46"/>
       <c r="Q77" s="45"/>
@@ -3217,7 +3217,7 @@
       <c r="C78" s="40"/>
       <c r="D78" s="41"/>
       <c r="E78" s="48"/>
-      <c r="F78" s="109"/>
+      <c r="F78" s="94"/>
       <c r="G78" s="49"/>
       <c r="H78" s="49"/>
       <c r="I78" s="49"/>
@@ -3225,7 +3225,7 @@
       <c r="K78" s="51"/>
       <c r="L78" s="45"/>
       <c r="M78" s="46"/>
-      <c r="N78" s="112"/>
+      <c r="N78" s="97"/>
       <c r="O78" s="47"/>
       <c r="P78" s="46"/>
       <c r="Q78" s="45"/>
@@ -3237,7 +3237,7 @@
       <c r="C79" s="40"/>
       <c r="D79" s="41"/>
       <c r="E79" s="48"/>
-      <c r="F79" s="109"/>
+      <c r="F79" s="94"/>
       <c r="G79" s="49"/>
       <c r="H79" s="49"/>
       <c r="I79" s="49"/>
@@ -3245,7 +3245,7 @@
       <c r="K79" s="51"/>
       <c r="L79" s="45"/>
       <c r="M79" s="46"/>
-      <c r="N79" s="112"/>
+      <c r="N79" s="97"/>
       <c r="O79" s="47"/>
       <c r="P79" s="46"/>
       <c r="Q79" s="45"/>
@@ -3257,7 +3257,7 @@
       <c r="C80" s="40"/>
       <c r="D80" s="41"/>
       <c r="E80" s="48"/>
-      <c r="F80" s="109"/>
+      <c r="F80" s="94"/>
       <c r="G80" s="49"/>
       <c r="H80" s="49"/>
       <c r="I80" s="49"/>
@@ -3265,7 +3265,7 @@
       <c r="K80" s="51"/>
       <c r="L80" s="45"/>
       <c r="M80" s="46"/>
-      <c r="N80" s="112"/>
+      <c r="N80" s="97"/>
       <c r="O80" s="47"/>
       <c r="P80" s="46"/>
       <c r="Q80" s="45"/>
@@ -3277,7 +3277,7 @@
       <c r="C81" s="40"/>
       <c r="D81" s="41"/>
       <c r="E81" s="48"/>
-      <c r="F81" s="109"/>
+      <c r="F81" s="94"/>
       <c r="G81" s="49"/>
       <c r="H81" s="49"/>
       <c r="I81" s="49"/>
@@ -3285,7 +3285,7 @@
       <c r="K81" s="51"/>
       <c r="L81" s="45"/>
       <c r="M81" s="46"/>
-      <c r="N81" s="112"/>
+      <c r="N81" s="97"/>
       <c r="O81" s="47"/>
       <c r="P81" s="46"/>
       <c r="Q81" s="45"/>
@@ -3297,7 +3297,7 @@
       <c r="C82" s="40"/>
       <c r="D82" s="41"/>
       <c r="E82" s="48"/>
-      <c r="F82" s="109"/>
+      <c r="F82" s="94"/>
       <c r="G82" s="49"/>
       <c r="H82" s="49"/>
       <c r="I82" s="49"/>
@@ -3305,7 +3305,7 @@
       <c r="K82" s="51"/>
       <c r="L82" s="45"/>
       <c r="M82" s="46"/>
-      <c r="N82" s="112"/>
+      <c r="N82" s="97"/>
       <c r="O82" s="47"/>
       <c r="P82" s="46"/>
       <c r="Q82" s="45"/>
@@ -3317,7 +3317,7 @@
       <c r="C83" s="40"/>
       <c r="D83" s="41"/>
       <c r="E83" s="48"/>
-      <c r="F83" s="109"/>
+      <c r="F83" s="94"/>
       <c r="G83" s="49"/>
       <c r="H83" s="49"/>
       <c r="I83" s="49"/>
@@ -3325,7 +3325,7 @@
       <c r="K83" s="51"/>
       <c r="L83" s="45"/>
       <c r="M83" s="46"/>
-      <c r="N83" s="112"/>
+      <c r="N83" s="97"/>
       <c r="O83" s="47"/>
       <c r="P83" s="46"/>
       <c r="Q83" s="45"/>
@@ -3337,7 +3337,7 @@
       <c r="C84" s="40"/>
       <c r="D84" s="41"/>
       <c r="E84" s="48"/>
-      <c r="F84" s="109"/>
+      <c r="F84" s="94"/>
       <c r="G84" s="49"/>
       <c r="H84" s="49"/>
       <c r="I84" s="49"/>
@@ -3345,7 +3345,7 @@
       <c r="K84" s="51"/>
       <c r="L84" s="45"/>
       <c r="M84" s="46"/>
-      <c r="N84" s="112"/>
+      <c r="N84" s="97"/>
       <c r="O84" s="47"/>
       <c r="P84" s="46"/>
       <c r="Q84" s="45"/>
@@ -3357,7 +3357,7 @@
       <c r="C85" s="40"/>
       <c r="D85" s="41"/>
       <c r="E85" s="48"/>
-      <c r="F85" s="109"/>
+      <c r="F85" s="94"/>
       <c r="G85" s="49"/>
       <c r="H85" s="49"/>
       <c r="I85" s="49"/>
@@ -3365,7 +3365,7 @@
       <c r="K85" s="51"/>
       <c r="L85" s="45"/>
       <c r="M85" s="46"/>
-      <c r="N85" s="112"/>
+      <c r="N85" s="97"/>
       <c r="O85" s="47"/>
       <c r="P85" s="46"/>
       <c r="Q85" s="45"/>
@@ -3377,7 +3377,7 @@
       <c r="C86" s="40"/>
       <c r="D86" s="41"/>
       <c r="E86" s="48"/>
-      <c r="F86" s="109"/>
+      <c r="F86" s="94"/>
       <c r="G86" s="49"/>
       <c r="H86" s="49"/>
       <c r="I86" s="49"/>
@@ -3385,7 +3385,7 @@
       <c r="K86" s="51"/>
       <c r="L86" s="45"/>
       <c r="M86" s="46"/>
-      <c r="N86" s="112"/>
+      <c r="N86" s="97"/>
       <c r="O86" s="47"/>
       <c r="P86" s="46"/>
       <c r="Q86" s="45"/>
@@ -3397,7 +3397,7 @@
       <c r="C87" s="40"/>
       <c r="D87" s="41"/>
       <c r="E87" s="48"/>
-      <c r="F87" s="109"/>
+      <c r="F87" s="94"/>
       <c r="G87" s="49"/>
       <c r="H87" s="49"/>
       <c r="I87" s="49"/>
@@ -3405,7 +3405,7 @@
       <c r="K87" s="51"/>
       <c r="L87" s="45"/>
       <c r="M87" s="46"/>
-      <c r="N87" s="112"/>
+      <c r="N87" s="97"/>
       <c r="O87" s="47"/>
       <c r="P87" s="46"/>
       <c r="Q87" s="45"/>
@@ -3417,7 +3417,7 @@
       <c r="C88" s="40"/>
       <c r="D88" s="41"/>
       <c r="E88" s="48"/>
-      <c r="F88" s="109"/>
+      <c r="F88" s="94"/>
       <c r="G88" s="49"/>
       <c r="H88" s="49"/>
       <c r="I88" s="49"/>
@@ -3425,7 +3425,7 @@
       <c r="K88" s="51"/>
       <c r="L88" s="45"/>
       <c r="M88" s="46"/>
-      <c r="N88" s="112"/>
+      <c r="N88" s="97"/>
       <c r="O88" s="47"/>
       <c r="P88" s="46"/>
       <c r="Q88" s="45"/>
@@ -3437,7 +3437,7 @@
       <c r="C89" s="40"/>
       <c r="D89" s="41"/>
       <c r="E89" s="48"/>
-      <c r="F89" s="109"/>
+      <c r="F89" s="94"/>
       <c r="G89" s="49"/>
       <c r="H89" s="49"/>
       <c r="I89" s="49"/>
@@ -3445,7 +3445,7 @@
       <c r="K89" s="51"/>
       <c r="L89" s="45"/>
       <c r="M89" s="46"/>
-      <c r="N89" s="112"/>
+      <c r="N89" s="97"/>
       <c r="O89" s="47"/>
       <c r="P89" s="46"/>
       <c r="Q89" s="45"/>
@@ -3457,7 +3457,7 @@
       <c r="C90" s="40"/>
       <c r="D90" s="41"/>
       <c r="E90" s="48"/>
-      <c r="F90" s="109"/>
+      <c r="F90" s="94"/>
       <c r="G90" s="49"/>
       <c r="H90" s="49"/>
       <c r="I90" s="49"/>
@@ -3465,7 +3465,7 @@
       <c r="K90" s="51"/>
       <c r="L90" s="45"/>
       <c r="M90" s="46"/>
-      <c r="N90" s="112"/>
+      <c r="N90" s="97"/>
       <c r="O90" s="47"/>
       <c r="P90" s="46"/>
       <c r="Q90" s="45"/>
@@ -3477,7 +3477,7 @@
       <c r="C91" s="40"/>
       <c r="D91" s="41"/>
       <c r="E91" s="48"/>
-      <c r="F91" s="109"/>
+      <c r="F91" s="94"/>
       <c r="G91" s="49"/>
       <c r="H91" s="49"/>
       <c r="I91" s="49"/>
@@ -3485,7 +3485,7 @@
       <c r="K91" s="51"/>
       <c r="L91" s="45"/>
       <c r="M91" s="46"/>
-      <c r="N91" s="112"/>
+      <c r="N91" s="97"/>
       <c r="O91" s="47"/>
       <c r="P91" s="46"/>
       <c r="Q91" s="45"/>
@@ -3497,7 +3497,7 @@
       <c r="C92" s="40"/>
       <c r="D92" s="41"/>
       <c r="E92" s="48"/>
-      <c r="F92" s="109"/>
+      <c r="F92" s="94"/>
       <c r="G92" s="49"/>
       <c r="H92" s="49"/>
       <c r="I92" s="49"/>
@@ -3505,7 +3505,7 @@
       <c r="K92" s="51"/>
       <c r="L92" s="45"/>
       <c r="M92" s="46"/>
-      <c r="N92" s="112"/>
+      <c r="N92" s="97"/>
       <c r="O92" s="47"/>
       <c r="P92" s="46"/>
       <c r="Q92" s="45"/>
@@ -3517,7 +3517,7 @@
       <c r="C93" s="40"/>
       <c r="D93" s="41"/>
       <c r="E93" s="48"/>
-      <c r="F93" s="109"/>
+      <c r="F93" s="94"/>
       <c r="G93" s="49"/>
       <c r="H93" s="49"/>
       <c r="I93" s="49"/>
@@ -3525,7 +3525,7 @@
       <c r="K93" s="51"/>
       <c r="L93" s="45"/>
       <c r="M93" s="46"/>
-      <c r="N93" s="112"/>
+      <c r="N93" s="97"/>
       <c r="O93" s="47"/>
       <c r="P93" s="46"/>
       <c r="Q93" s="45"/>
@@ -3537,7 +3537,7 @@
       <c r="C94" s="40"/>
       <c r="D94" s="41"/>
       <c r="E94" s="48"/>
-      <c r="F94" s="109"/>
+      <c r="F94" s="94"/>
       <c r="G94" s="49"/>
       <c r="H94" s="49"/>
       <c r="I94" s="49"/>
@@ -3545,7 +3545,7 @@
       <c r="K94" s="51"/>
       <c r="L94" s="45"/>
       <c r="M94" s="46"/>
-      <c r="N94" s="112"/>
+      <c r="N94" s="97"/>
       <c r="O94" s="47"/>
       <c r="P94" s="46"/>
       <c r="Q94" s="45"/>
@@ -3557,7 +3557,7 @@
       <c r="C95" s="40"/>
       <c r="D95" s="41"/>
       <c r="E95" s="48"/>
-      <c r="F95" s="109"/>
+      <c r="F95" s="94"/>
       <c r="G95" s="49"/>
       <c r="H95" s="49"/>
       <c r="I95" s="49"/>
@@ -3565,7 +3565,7 @@
       <c r="K95" s="51"/>
       <c r="L95" s="45"/>
       <c r="M95" s="46"/>
-      <c r="N95" s="112"/>
+      <c r="N95" s="97"/>
       <c r="O95" s="47"/>
       <c r="P95" s="46"/>
       <c r="Q95" s="45"/>
@@ -3577,7 +3577,7 @@
       <c r="C96" s="40"/>
       <c r="D96" s="41"/>
       <c r="E96" s="48"/>
-      <c r="F96" s="109"/>
+      <c r="F96" s="94"/>
       <c r="G96" s="49"/>
       <c r="H96" s="49"/>
       <c r="I96" s="49"/>
@@ -3585,7 +3585,7 @@
       <c r="K96" s="51"/>
       <c r="L96" s="45"/>
       <c r="M96" s="46"/>
-      <c r="N96" s="112"/>
+      <c r="N96" s="97"/>
       <c r="O96" s="47"/>
       <c r="P96" s="46"/>
       <c r="Q96" s="45"/>
@@ -3597,7 +3597,7 @@
       <c r="C97" s="40"/>
       <c r="D97" s="41"/>
       <c r="E97" s="48"/>
-      <c r="F97" s="109"/>
+      <c r="F97" s="94"/>
       <c r="G97" s="49"/>
       <c r="H97" s="49"/>
       <c r="I97" s="49"/>
@@ -3605,7 +3605,7 @@
       <c r="K97" s="51"/>
       <c r="L97" s="45"/>
       <c r="M97" s="46"/>
-      <c r="N97" s="112"/>
+      <c r="N97" s="97"/>
       <c r="O97" s="47"/>
       <c r="P97" s="46"/>
       <c r="Q97" s="45"/>
@@ -3617,7 +3617,7 @@
       <c r="C98" s="40"/>
       <c r="D98" s="41"/>
       <c r="E98" s="48"/>
-      <c r="F98" s="109"/>
+      <c r="F98" s="94"/>
       <c r="G98" s="49"/>
       <c r="H98" s="49"/>
       <c r="I98" s="49"/>
@@ -3625,7 +3625,7 @@
       <c r="K98" s="51"/>
       <c r="L98" s="45"/>
       <c r="M98" s="46"/>
-      <c r="N98" s="112"/>
+      <c r="N98" s="97"/>
       <c r="O98" s="47"/>
       <c r="P98" s="46"/>
       <c r="Q98" s="45"/>
@@ -3637,7 +3637,7 @@
       <c r="C99" s="40"/>
       <c r="D99" s="41"/>
       <c r="E99" s="48"/>
-      <c r="F99" s="109"/>
+      <c r="F99" s="94"/>
       <c r="G99" s="49"/>
       <c r="H99" s="49"/>
       <c r="I99" s="49"/>
@@ -3645,7 +3645,7 @@
       <c r="K99" s="51"/>
       <c r="L99" s="45"/>
       <c r="M99" s="46"/>
-      <c r="N99" s="112"/>
+      <c r="N99" s="97"/>
       <c r="O99" s="47"/>
       <c r="P99" s="46"/>
       <c r="Q99" s="45"/>
@@ -3657,7 +3657,7 @@
       <c r="C100" s="40"/>
       <c r="D100" s="41"/>
       <c r="E100" s="48"/>
-      <c r="F100" s="109"/>
+      <c r="F100" s="94"/>
       <c r="G100" s="49"/>
       <c r="H100" s="49"/>
       <c r="I100" s="49"/>
@@ -3665,7 +3665,7 @@
       <c r="K100" s="51"/>
       <c r="L100" s="45"/>
       <c r="M100" s="46"/>
-      <c r="N100" s="112"/>
+      <c r="N100" s="97"/>
       <c r="O100" s="47"/>
       <c r="P100" s="46"/>
       <c r="Q100" s="45"/>
@@ -3677,7 +3677,7 @@
       <c r="C101" s="40"/>
       <c r="D101" s="41"/>
       <c r="E101" s="48"/>
-      <c r="F101" s="109"/>
+      <c r="F101" s="94"/>
       <c r="G101" s="49"/>
       <c r="H101" s="49"/>
       <c r="I101" s="49"/>
@@ -3685,7 +3685,7 @@
       <c r="K101" s="51"/>
       <c r="L101" s="45"/>
       <c r="M101" s="46"/>
-      <c r="N101" s="112"/>
+      <c r="N101" s="97"/>
       <c r="O101" s="47"/>
       <c r="P101" s="46"/>
       <c r="Q101" s="45"/>
@@ -3697,7 +3697,7 @@
       <c r="C102" s="52"/>
       <c r="D102" s="53"/>
       <c r="E102" s="54"/>
-      <c r="F102" s="110"/>
+      <c r="F102" s="95"/>
       <c r="G102" s="55"/>
       <c r="H102" s="55"/>
       <c r="I102" s="55"/>
@@ -3705,7 +3705,7 @@
       <c r="K102" s="57"/>
       <c r="L102" s="58"/>
       <c r="M102" s="59"/>
-      <c r="N102" s="113"/>
+      <c r="N102" s="98"/>
       <c r="O102" s="60"/>
       <c r="P102" s="59"/>
       <c r="Q102" s="58"/>
@@ -3722,8 +3722,8 @@
     <mergeCell ref="F1:H1"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid concentration" error="1-30ng/µl is required for DNA samples. Leave blank for strains." prompt="1-30ng/µl is required for DNA samples. Leave blank for strains." sqref="D7:D102">
-      <formula1>1</formula1>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid concentration" error="1-30ng/µl is required for DNA samples. Leave blank for strains." prompt="0-30ng/µl is required for DNA samples. Leave blank for strains." sqref="D7:D102">
+      <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid volume" error="30-100µl volume is required for DNA samples. Leave blank for strains." prompt="30-100µl volume is required for DNA samples. Leave blank for strains." sqref="E7:E102">

</xml_diff>